<commit_message>
Added two labels that were still missing
</commit_message>
<xml_diff>
--- a/data/llm_correction_check/llm_correction_checked_1.1.xlsx
+++ b/data/llm_correction_check/llm_correction_checked_1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumente\GitHub Desktop\nonsig-master-thesis\data\llm_correction_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6CD1D5-C038-4EA2-8056-2EFD551B64F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237084F6-55CF-4F00-A0B0-288DCD42B14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
+    <workbookView xWindow="-28920" yWindow="3015" windowWidth="29040" windowHeight="15720" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="llm_correction_checked" sheetId="1" r:id="rId1"/>
@@ -1656,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,7 +2109,9 @@
       <c r="C29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
       <c r="E29" s="4" t="s">
         <v>205</v>
       </c>
@@ -2124,7 +2126,9 @@
       <c r="C30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
       <c r="E30" s="4" t="s">
         <v>205</v>
       </c>

</xml_diff>